<commit_message>
updated in-game pause menu; mainmenu shouldn't be saved as 'room' to load into
</commit_message>
<xml_diff>
--- a/assets/list of sounds.xlsx
+++ b/assets/list of sounds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roosevelt\Documents\GameMakerStudio2\diver-man\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D833FE84-2755-4468-85D6-69DFDDB6A60A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C326FE80-12B4-4C66-BED9-BFAA96D8FA53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E1050BD-5518-40D0-868A-97AEDB9BBE8C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5E1050BD-5518-40D0-868A-97AEDB9BBE8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>out of water</t>
   </si>
@@ -33,9 +33,6 @@
     <t>in water</t>
   </si>
   <si>
-    <t>footsteps on wood</t>
-  </si>
-  <si>
     <t>crane lowering</t>
   </si>
   <si>
@@ -64,6 +61,36 @@
   </si>
   <si>
     <t>knocking into bush</t>
+  </si>
+  <si>
+    <t>footsteps on pavement</t>
+  </si>
+  <si>
+    <t>seagulls</t>
+  </si>
+  <si>
+    <t>voices</t>
+  </si>
+  <si>
+    <t>brother</t>
+  </si>
+  <si>
+    <t>sailor pete</t>
+  </si>
+  <si>
+    <t>bully1</t>
+  </si>
+  <si>
+    <t>bully2</t>
+  </si>
+  <si>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>vendors daughter</t>
+  </si>
+  <si>
+    <t>rock being smacked</t>
   </si>
 </sst>
 </file>
@@ -431,19 +458,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D516E081-9126-4E7D-B457-10C2C9C93FDE}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -451,50 +479,79 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
music; bob ross; new build
</commit_message>
<xml_diff>
--- a/assets/list of sounds.xlsx
+++ b/assets/list of sounds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roosevelt\Documents\GameMakerStudio2\diver-man\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C326FE80-12B4-4C66-BED9-BFAA96D8FA53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB5F150-A714-4785-A701-00D63F102999}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5E1050BD-5518-40D0-868A-97AEDB9BBE8C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>out of water</t>
   </si>
@@ -87,10 +87,13 @@
     <t>vendor</t>
   </si>
   <si>
-    <t>vendors daughter</t>
-  </si>
-  <si>
     <t>rock being smacked</t>
+  </si>
+  <si>
+    <t>bob ross</t>
+  </si>
+  <si>
+    <t>nadya</t>
   </si>
 </sst>
 </file>
@@ -114,7 +117,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +127,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -140,10 +149,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D516E081-9126-4E7D-B457-10C2C9C93FDE}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +505,7 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -514,7 +524,7 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
@@ -525,7 +535,7 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
@@ -548,10 +558,15 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>